<commit_message>
T1: Obliczona gestosc, rozpoczete liczenie niepewnosci gestosci , poprawiony blad z Pi w niepewnosci tuleji, wklejona niepewnosc do glownego archiwum
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/Objetosc Tulejka.xlsx
+++ b/Fizyka_Sprawka/Objetosc Tulejka.xlsx
@@ -2650,7 +2650,6 @@
               <a:endParaRPr lang="pl-PL" sz="1100"/>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:r>
@@ -3243,7 +3242,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3259,7 +3258,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3272,7 +3271,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3314,7 +3313,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3363,7 +3362,7 @@
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
-                            <m:t>-</m:t>
+                            <m:t>−</m:t>
                           </m:r>
                           <m:r>
                             <m:rPr>
@@ -3424,7 +3423,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3438,7 +3437,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3452,7 +3451,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3465,7 +3464,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3507,7 +3506,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3556,7 +3555,7 @@
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
-                            <m:t>-</m:t>
+                            <m:t>−</m:t>
                           </m:r>
                           <m:r>
                             <m:rPr>
@@ -3611,7 +3610,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3625,7 +3624,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3639,7 +3638,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3664,7 +3663,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3743,7 +3742,7 @@
                                 <a:schemeClr val="tx1"/>
                               </a:solidFill>
                               <a:effectLst/>
-                              <a:latin typeface="+mn-lt"/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               <a:ea typeface="+mn-ea"/>
                               <a:cs typeface="+mn-cs"/>
                             </a:rPr>
@@ -3798,7 +3797,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3821,6 +3820,49 @@
                         </a:rPr>
                         <m:t>61982.38616</m:t>
                       </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝜋</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>2</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSup>
                       <m:r>
                         <m:rPr>
                           <m:nor/>
@@ -3834,7 +3876,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3855,6 +3897,49 @@
                         </a:rPr>
                         <m:t>61982.38616</m:t>
                       </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝜋</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>2</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSup>
                       <m:r>
                         <m:rPr>
                           <m:nor/>
@@ -3868,7 +3953,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3889,6 +3974,49 @@
                         </a:rPr>
                         <m:t>176.1313586</m:t>
                       </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="pl-PL" sz="1100" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝜋</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>2</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSup>
                       <m:r>
                         <m:rPr>
                           <m:nor/>
@@ -3919,7 +4047,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -3942,6 +4070,49 @@
                         </a:rPr>
                         <m:t>124140.9037</m:t>
                       </m:r>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝜋</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                              <a:solidFill>
+                                <a:schemeClr val="tx1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>2</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSup>
                       <m:r>
                         <m:rPr>
                           <m:nor/>
@@ -3957,7 +4128,7 @@
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -3977,6 +4148,22 @@
                 </a:rPr>
                 <a:t>352.3363502</a:t>
               </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
               <a:r>
                 <a:rPr lang="en-US"/>
                 <a:t> </a:t>
@@ -3998,12 +4185,23 @@
                 </a:rPr>
                 <a:t>360</a:t>
               </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="pl-PL" i="1">
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝜋</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
               <a:endParaRPr lang="en-US">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
           </xdr:txBody>
@@ -4252,7 +4450,6 @@
               <a:endParaRPr lang="pl-PL" sz="1100"/>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:solidFill>
@@ -4523,14 +4720,38 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>√(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>〖(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>√(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4539,7 +4760,31 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>〖("</a:t>
+                <a:t>2h</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" 𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pl-PL" sz="1100" i="0">
@@ -4551,6 +4796,48 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>(dwew−dzew)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:effectLst/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" )〗^2+〖(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
                 <a:t>2h</a:t>
               </a:r>
               <a:r>
@@ -4559,11 +4846,23 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" 𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" 𝜋"</a:t>
+                <a:t>"</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pl-PL" sz="1100" i="0">
@@ -4575,25 +4874,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>(dwew-dzew)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" i="0">
-                  <a:effectLst/>
-                </a:rPr>
-                <a:t> </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>" )</a:t>
+                <a:t>(dzew−dwew)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
@@ -4605,115 +4886,19 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>〗^2+〖("</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>2h</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>" 𝜋"</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>(dzew-dwew)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>)" 〗^2+〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>𝜋</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>(𝑑𝑧𝑒𝑤−𝑑𝑤𝑒𝑤))</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>〗^2</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>=</a:t>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" 〗^2+〖(𝜋(𝑑𝑧𝑒𝑤−𝑑𝑤𝑒𝑤))〗^2=</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
@@ -4721,7 +4906,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -4753,11 +4938,23 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>√(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>√(</a:t>
+                <a:t>"61982.38616</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -4765,11 +4962,35 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>"61982.38616</a:t>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>^2 "</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" i="0"/>
@@ -4781,11 +5002,23 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" +</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" +</a:t>
+                <a:t>"61982.38616</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -4793,11 +5026,35 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>"61982.38616</a:t>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>^2 "</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" i="0"/>
@@ -4809,11 +5066,23 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" +</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" +</a:t>
+                <a:t>"176.1313586</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -4821,18 +5090,84 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>"176.1313586</a:t>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>^2 "</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" i="0"/>
                 <a:t> </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>√(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4841,83 +5176,89 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
+                <a:t>"124140.9037</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
                 <a:t>" </a:t>
               </a:r>
               <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>=</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>√(</a:t>
-              </a:r>
-              <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>"124140.9037</a:t>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜋</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>^2 "</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" i="0"/>
                 <a:t> </a:t>
               </a:r>
               <a:r>
+                <a:rPr lang="en-US" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" )</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="pl-PL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>=</a:t>
+                <a:t>352.3363502</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
@@ -4925,11 +5266,11 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>352.3363502</a:t>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜋</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US"/>
@@ -4947,13 +5288,20 @@
                   <a:effectLst/>
                 </a:rPr>
                 <a:t>360</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="pl-PL" i="0">
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜋</a:t>
               </a:r>
               <a:endParaRPr lang="en-US">
                 <a:effectLst/>
               </a:endParaRPr>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
           </xdr:txBody>
@@ -7914,8 +8262,8 @@
       <xdr:rowOff>2839</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3205843" cy="419154"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="TextBox 20"/>
@@ -8135,7 +8483,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="21" name="TextBox 20"/>
@@ -8283,8 +8631,8 @@
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2455416" cy="246927"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="TextBox 23"/>
@@ -8587,7 +8935,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="24" name="TextBox 23"/>
@@ -8979,8 +9327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Z40" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>